<commit_message>
Atualização automática de PORTO_ALEGRE.xlsx
</commit_message>
<xml_diff>
--- a/PORTO_ALEGRE.xlsx
+++ b/PORTO_ALEGRE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B92804BF-17D0-46CB-9E0A-C541D78896A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61AB286E-286D-4E0E-89DE-5D54F433614D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -2435,7 +2422,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{169BBDFE-0719-4390-BC2D-34E59FB875C0}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{FE6DA7E5-A740-45E3-9B51-265902F6A432}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2465,10 +2452,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27AB5224-A22E-4D8C-A496-1D55784D90AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40A036BC-1AE5-4FF9-B80F-1354CA1EAF7B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2506,7 +2493,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6995DB6C-994B-48EC-B8B7-3243E097918B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E08DCB42-A619-43D2-A39C-604E8CE38C70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2569,7 +2556,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9298AC5-7173-4EE6-9573-E13586EFA278}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E472B15B-F101-4A75-A943-0307B3F34E38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2588,7 +2575,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10777874-361A-5E44-ABFB-1EA72B837D5F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{811F197A-F909-2596-4607-DBF6DE062ABE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2637,7 +2624,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56425ECC-89AD-084F-6B8C-60B8375BDDEA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6D43E39-444C-5EC0-2A60-7328E1814723}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2656,7 +2643,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4460E867-F327-DD9A-D656-5A0261B7E4A1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32FF775-23AE-BB00-D658-FBA4C945CA2D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2687,7 +2674,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B718C1BE-B23A-B44A-F5AC-E0C3C7764DF7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B89EC777-3C6A-0667-69B8-0EDB8530197B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2718,7 +2705,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C62143-68D9-5F90-CEFF-66DC4D87CEE4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBE7EDEC-8AA8-0F6D-4A19-E543CB2D6270}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2761,7 +2748,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DD1CC88-9B10-4EF5-A486-1CDEFA6C7527}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33C0B0C5-A97B-43BA-81B6-7E8CDC6F0A79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2799,7 +2786,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0AD9731-657D-4E1F-87F2-4BD7693E3B2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3278ABC-D633-4412-8577-ABD5183AA980}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2842,7 +2829,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96CDCA29-832F-4078-82D4-D924F39F4878}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39E7D058-D34C-4340-ACB6-57E245330723}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3155,7 +3142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671071ED-A2C0-432E-BB4D-484522F6619B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76A6918-263F-4D7B-B19F-CBFECCD3FE75}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10910,7 +10897,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11458,16 +11445,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17721,8 +17708,9 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17828,8 +17816,7 @@
         <v>687</v>
       </c>
       <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
-        <v>2663</v>
+        <v>15072</v>
       </c>
       <c r="F1" s="36">
         <v>1</v>

</xml_diff>